<commit_message>
allocation tables now have [of Coal mines]
</commit_message>
<xml_diff>
--- a/inst/extdata/GH-ZA-Allocation-sample-2018.xlsx
+++ b/inst/extdata/GH-ZA-Allocation-sample-2018.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/IEATools/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/IEATools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06AA538-01E1-1E48-842F-8516BEB53A56}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372FB98D-DC09-7242-8768-1CE551122534}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FU Allocations" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7279" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7289" uniqueCount="118">
   <si>
     <t>Country</t>
   </si>
@@ -190,13 +198,7 @@
     <t>Gas works gas</t>
   </si>
   <si>
-    <t>Hard coal (if no detail) (Coal mines)</t>
-  </si>
-  <si>
     <t>Iron and steel</t>
-  </si>
-  <si>
-    <t>Other bituminous coal (Coal mines)</t>
   </si>
   <si>
     <t>Coke oven coke</t>
@@ -374,6 +376,12 @@
   </si>
   <si>
     <t>Wood furnaces</t>
+  </si>
+  <si>
+    <t>Hard coal (if no detail) [of Coal mines]</t>
+  </si>
+  <si>
+    <t>Other bituminous coal [of Coal mines]</t>
   </si>
 </sst>
 </file>
@@ -746,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O692"/>
+  <dimension ref="A1:O693"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
-      <selection activeCell="N235" sqref="N235:O236"/>
+    <sheetView tabSelected="1" topLeftCell="A641" workbookViewId="0">
+      <selection activeCell="L693" sqref="L693"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -929,10 +937,10 @@
         <v>22</v>
       </c>
       <c r="I4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K4" t="s">
         <v>23</v>
@@ -1126,10 +1134,10 @@
         <v>29</v>
       </c>
       <c r="I9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K9" t="s">
         <v>30</v>
@@ -1171,10 +1179,10 @@
         <v>29</v>
       </c>
       <c r="I10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K10" t="s">
         <v>30</v>
@@ -1331,10 +1339,10 @@
         <v>29</v>
       </c>
       <c r="I14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K14" t="s">
         <v>33</v>
@@ -1374,10 +1382,10 @@
         <v>29</v>
       </c>
       <c r="I15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K15" t="s">
         <v>33</v>
@@ -1533,10 +1541,10 @@
         <v>29</v>
       </c>
       <c r="I19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K19" t="s">
         <v>34</v>
@@ -1576,10 +1584,10 @@
         <v>29</v>
       </c>
       <c r="I20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K20" t="s">
         <v>34</v>
@@ -1735,10 +1743,10 @@
         <v>29</v>
       </c>
       <c r="I24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K24" t="s">
         <v>35</v>
@@ -1778,10 +1786,10 @@
         <v>29</v>
       </c>
       <c r="I25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J25" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K25" t="s">
         <v>35</v>
@@ -1821,10 +1829,10 @@
         <v>29</v>
       </c>
       <c r="I26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K26" t="s">
         <v>35</v>
@@ -1946,10 +1954,10 @@
         <v>36</v>
       </c>
       <c r="I29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J29" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K29" t="s">
         <v>37</v>
@@ -2139,10 +2147,10 @@
         <v>38</v>
       </c>
       <c r="I34" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J34" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K34" t="s">
         <v>37</v>
@@ -2336,10 +2344,10 @@
         <v>39</v>
       </c>
       <c r="I39" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J39" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K39" t="s">
         <v>37</v>
@@ -2533,10 +2541,10 @@
         <v>40</v>
       </c>
       <c r="I44" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J44" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K44" t="s">
         <v>37</v>
@@ -2730,10 +2738,10 @@
         <v>41</v>
       </c>
       <c r="I49" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J49" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K49" t="s">
         <v>37</v>
@@ -2927,10 +2935,10 @@
         <v>29</v>
       </c>
       <c r="I54" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J54" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K54" t="s">
         <v>37</v>
@@ -2972,10 +2980,10 @@
         <v>29</v>
       </c>
       <c r="I55" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J55" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K55" t="s">
         <v>37</v>
@@ -3017,10 +3025,10 @@
         <v>29</v>
       </c>
       <c r="I56" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J56" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K56" t="s">
         <v>37</v>
@@ -3148,10 +3156,10 @@
         <v>43</v>
       </c>
       <c r="I59" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J59" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K59" t="s">
         <v>44</v>
@@ -3345,10 +3353,10 @@
         <v>39</v>
       </c>
       <c r="I64" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J64" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K64" t="s">
         <v>44</v>
@@ -3390,10 +3398,10 @@
         <v>39</v>
       </c>
       <c r="I65" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J65" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K65" t="s">
         <v>44</v>
@@ -3554,10 +3562,10 @@
         <v>39</v>
       </c>
       <c r="I69" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J69" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K69" t="s">
         <v>45</v>
@@ -3747,10 +3755,10 @@
         <v>40</v>
       </c>
       <c r="I74" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J74" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K74" t="s">
         <v>45</v>
@@ -3944,10 +3952,10 @@
         <v>39</v>
       </c>
       <c r="I79" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J79" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K79" t="s">
         <v>46</v>
@@ -4137,10 +4145,10 @@
         <v>40</v>
       </c>
       <c r="I84" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J84" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K84" t="s">
         <v>46</v>
@@ -4334,10 +4342,10 @@
         <v>36</v>
       </c>
       <c r="I89" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J89" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K89" t="s">
         <v>48</v>
@@ -4531,10 +4539,10 @@
         <v>38</v>
       </c>
       <c r="I94" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J94" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K94" t="s">
         <v>48</v>
@@ -4728,10 +4736,10 @@
         <v>41</v>
       </c>
       <c r="I99" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J99" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K99" t="s">
         <v>48</v>
@@ -4925,10 +4933,10 @@
         <v>49</v>
       </c>
       <c r="I104" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J104" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K104" t="s">
         <v>48</v>
@@ -5122,10 +5130,10 @@
         <v>29</v>
       </c>
       <c r="I109" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J109" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K109" t="s">
         <v>48</v>
@@ -5167,10 +5175,10 @@
         <v>29</v>
       </c>
       <c r="I110" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J110" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K110" t="s">
         <v>48</v>
@@ -5212,10 +5220,10 @@
         <v>29</v>
       </c>
       <c r="I111" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J111" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K111" t="s">
         <v>48</v>
@@ -5257,16 +5265,16 @@
         <v>29</v>
       </c>
       <c r="I112" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J112" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K112" t="s">
         <v>48</v>
       </c>
       <c r="L112" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M112" s="3"/>
       <c r="N112" s="6">
@@ -5384,10 +5392,10 @@
         <v>36</v>
       </c>
       <c r="I115" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J115" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K115" t="s">
         <v>50</v>
@@ -5577,10 +5585,10 @@
         <v>39</v>
       </c>
       <c r="I120" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J120" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K120" t="s">
         <v>50</v>
@@ -5770,10 +5778,10 @@
         <v>41</v>
       </c>
       <c r="I125" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J125" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K125" t="s">
         <v>50</v>
@@ -5967,10 +5975,10 @@
         <v>29</v>
       </c>
       <c r="I130" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J130" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K130" t="s">
         <v>50</v>
@@ -6164,10 +6172,10 @@
         <v>39</v>
       </c>
       <c r="I135" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J135" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K135" t="s">
         <v>51</v>
@@ -6209,10 +6217,10 @@
         <v>39</v>
       </c>
       <c r="I136" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J136" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K136" t="s">
         <v>51</v>
@@ -6369,10 +6377,10 @@
         <v>41</v>
       </c>
       <c r="I140" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J140" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K140" t="s">
         <v>51</v>
@@ -6562,10 +6570,10 @@
         <v>29</v>
       </c>
       <c r="I145" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J145" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K145" t="s">
         <v>51</v>
@@ -6605,10 +6613,10 @@
         <v>29</v>
       </c>
       <c r="I146" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J146" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K146" t="s">
         <v>51</v>
@@ -6764,10 +6772,10 @@
         <v>43</v>
       </c>
       <c r="I150" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J150" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K150" t="s">
         <v>52</v>
@@ -6961,10 +6969,10 @@
         <v>29</v>
       </c>
       <c r="I155" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J155" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K155" t="s">
         <v>54</v>
@@ -7006,10 +7014,10 @@
         <v>29</v>
       </c>
       <c r="I156" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J156" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K156" t="s">
         <v>54</v>
@@ -7166,10 +7174,10 @@
         <v>55</v>
       </c>
       <c r="I160" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J160" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K160" t="s">
         <v>23</v>
@@ -7209,10 +7217,10 @@
         <v>55</v>
       </c>
       <c r="I161" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J161" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K161" t="s">
         <v>23</v>
@@ -7368,10 +7376,10 @@
         <v>22</v>
       </c>
       <c r="I165" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J165" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K165" t="s">
         <v>23</v>
@@ -7561,10 +7569,10 @@
         <v>40</v>
       </c>
       <c r="I170" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J170" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K170" t="s">
         <v>23</v>
@@ -7754,10 +7762,10 @@
         <v>29</v>
       </c>
       <c r="I175" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J175" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K175" t="s">
         <v>23</v>
@@ -7797,10 +7805,10 @@
         <v>29</v>
       </c>
       <c r="I176" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J176" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K176" t="s">
         <v>23</v>
@@ -7960,10 +7968,10 @@
         <v>29</v>
       </c>
       <c r="I180" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J180" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K180" t="s">
         <v>30</v>
@@ -8068,12 +8076,12 @@
         <v>21</v>
       </c>
       <c r="H183" s="1" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I183" s="1"/>
       <c r="J183" s="1"/>
       <c r="K183" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L183" s="1" t="s">
         <v>24</v>
@@ -8109,12 +8117,12 @@
         <v>21</v>
       </c>
       <c r="H184" s="1" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I184" s="1"/>
       <c r="J184" s="1"/>
       <c r="K184" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L184" s="1" t="s">
         <v>25</v>
@@ -8150,16 +8158,16 @@
         <v>21</v>
       </c>
       <c r="H185" t="s">
+        <v>116</v>
+      </c>
+      <c r="I185" t="s">
+        <v>80</v>
+      </c>
+      <c r="J185" t="s">
+        <v>75</v>
+      </c>
+      <c r="K185" t="s">
         <v>56</v>
-      </c>
-      <c r="I185" t="s">
-        <v>82</v>
-      </c>
-      <c r="J185" t="s">
-        <v>77</v>
-      </c>
-      <c r="K185" t="s">
-        <v>57</v>
       </c>
       <c r="L185" t="s">
         <v>26</v>
@@ -8193,10 +8201,10 @@
         <v>21</v>
       </c>
       <c r="H186" t="s">
+        <v>116</v>
+      </c>
+      <c r="K186" t="s">
         <v>56</v>
-      </c>
-      <c r="K186" t="s">
-        <v>57</v>
       </c>
       <c r="L186" t="s">
         <v>27</v>
@@ -8227,10 +8235,10 @@
         <v>21</v>
       </c>
       <c r="H187" t="s">
+        <v>116</v>
+      </c>
+      <c r="K187" t="s">
         <v>56</v>
-      </c>
-      <c r="K187" t="s">
-        <v>57</v>
       </c>
       <c r="L187" t="s">
         <v>28</v>
@@ -8261,12 +8269,12 @@
         <v>21</v>
       </c>
       <c r="H188" s="1" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I188" s="1"/>
       <c r="J188" s="1"/>
       <c r="K188" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L188" s="1" t="s">
         <v>24</v>
@@ -8302,12 +8310,12 @@
         <v>21</v>
       </c>
       <c r="H189" s="1" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I189" s="1"/>
       <c r="J189" s="1"/>
       <c r="K189" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L189" s="1" t="s">
         <v>25</v>
@@ -8343,16 +8351,16 @@
         <v>21</v>
       </c>
       <c r="H190" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I190" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J190" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K190" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L190" t="s">
         <v>26</v>
@@ -8386,10 +8394,10 @@
         <v>21</v>
       </c>
       <c r="H191" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="K191" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L191" t="s">
         <v>27</v>
@@ -8420,10 +8428,10 @@
         <v>21</v>
       </c>
       <c r="H192" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="K192" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L192" t="s">
         <v>28</v>
@@ -8454,12 +8462,12 @@
         <v>21</v>
       </c>
       <c r="H193" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I193" s="1"/>
       <c r="J193" s="1"/>
       <c r="K193" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L193" s="1" t="s">
         <v>24</v>
@@ -8497,12 +8505,12 @@
         <v>21</v>
       </c>
       <c r="H194" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I194" s="1"/>
       <c r="J194" s="1"/>
       <c r="K194" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L194" s="1" t="s">
         <v>25</v>
@@ -8540,16 +8548,16 @@
         <v>21</v>
       </c>
       <c r="H195" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I195" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J195" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K195" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L195" t="s">
         <v>26</v>
@@ -8585,10 +8593,10 @@
         <v>21</v>
       </c>
       <c r="H196" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K196" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L196" t="s">
         <v>27</v>
@@ -8618,10 +8626,10 @@
         <v>21</v>
       </c>
       <c r="H197" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K197" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L197" t="s">
         <v>28</v>
@@ -8656,7 +8664,7 @@
       <c r="I198" s="1"/>
       <c r="J198" s="1"/>
       <c r="K198" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L198" s="1" t="s">
         <v>24</v>
@@ -8699,7 +8707,7 @@
       <c r="I199" s="1"/>
       <c r="J199" s="1"/>
       <c r="K199" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L199" s="1" t="s">
         <v>25</v>
@@ -8740,13 +8748,13 @@
         <v>55</v>
       </c>
       <c r="I200" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J200" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K200" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L200" t="s">
         <v>26</v>
@@ -8785,7 +8793,7 @@
         <v>55</v>
       </c>
       <c r="K201" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L201" t="s">
         <v>27</v>
@@ -8818,7 +8826,7 @@
         <v>55</v>
       </c>
       <c r="K202" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L202" t="s">
         <v>28</v>
@@ -8848,12 +8856,12 @@
         <v>21</v>
       </c>
       <c r="H203" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I203" s="1"/>
       <c r="J203" s="1"/>
       <c r="K203" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L203" s="1" t="s">
         <v>24</v>
@@ -8891,12 +8899,12 @@
         <v>21</v>
       </c>
       <c r="H204" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I204" s="1"/>
       <c r="J204" s="1"/>
       <c r="K204" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L204" s="1" t="s">
         <v>25</v>
@@ -8934,16 +8942,16 @@
         <v>21</v>
       </c>
       <c r="H205" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I205" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J205" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K205" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L205" t="s">
         <v>26</v>
@@ -8979,10 +8987,10 @@
         <v>21</v>
       </c>
       <c r="H206" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K206" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L206" t="s">
         <v>27</v>
@@ -9012,10 +9020,10 @@
         <v>21</v>
       </c>
       <c r="H207" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K207" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L207" t="s">
         <v>28</v>
@@ -9045,12 +9053,12 @@
         <v>21</v>
       </c>
       <c r="H208" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I208" s="1"/>
       <c r="J208" s="1"/>
       <c r="K208" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L208" s="1" t="s">
         <v>24</v>
@@ -9088,12 +9096,12 @@
         <v>21</v>
       </c>
       <c r="H209" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I209" s="1"/>
       <c r="J209" s="1"/>
       <c r="K209" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L209" s="1" t="s">
         <v>25</v>
@@ -9131,16 +9139,16 @@
         <v>21</v>
       </c>
       <c r="H210" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I210" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J210" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K210" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L210" t="s">
         <v>26</v>
@@ -9176,10 +9184,10 @@
         <v>21</v>
       </c>
       <c r="H211" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K211" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L211" t="s">
         <v>27</v>
@@ -9209,10 +9217,10 @@
         <v>21</v>
       </c>
       <c r="H212" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K212" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L212" t="s">
         <v>28</v>
@@ -9247,7 +9255,7 @@
       <c r="I213" s="1"/>
       <c r="J213" s="1"/>
       <c r="K213" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L213" s="1" t="s">
         <v>24</v>
@@ -9290,7 +9298,7 @@
       <c r="I214" s="1"/>
       <c r="J214" s="1"/>
       <c r="K214" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L214" s="1" t="s">
         <v>25</v>
@@ -9331,13 +9339,13 @@
         <v>29</v>
       </c>
       <c r="I215" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J215" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K215" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L215" t="s">
         <v>26</v>
@@ -9376,13 +9384,13 @@
         <v>29</v>
       </c>
       <c r="I216" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J216" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K216" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L216" t="s">
         <v>27</v>
@@ -9421,13 +9429,13 @@
         <v>29</v>
       </c>
       <c r="I217" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J217" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K217" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L217" t="s">
         <v>28</v>
@@ -9463,12 +9471,12 @@
         <v>21</v>
       </c>
       <c r="H218" s="1" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I218" s="1"/>
       <c r="J218" s="1"/>
       <c r="K218" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L218" s="1" t="s">
         <v>24</v>
@@ -9504,12 +9512,12 @@
         <v>21</v>
       </c>
       <c r="H219" s="1" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I219" s="1"/>
       <c r="J219" s="1"/>
       <c r="K219" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L219" s="1" t="s">
         <v>25</v>
@@ -9545,16 +9553,16 @@
         <v>21</v>
       </c>
       <c r="H220" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I220" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J220" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K220" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L220" t="s">
         <v>26</v>
@@ -9588,16 +9596,16 @@
         <v>21</v>
       </c>
       <c r="H221" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I221" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J221" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K221" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L221" t="s">
         <v>27</v>
@@ -9631,10 +9639,10 @@
         <v>21</v>
       </c>
       <c r="H222" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="K222" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L222" t="s">
         <v>28</v>
@@ -9670,7 +9678,7 @@
       <c r="I223" s="1"/>
       <c r="J223" s="1"/>
       <c r="K223" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L223" s="1" t="s">
         <v>24</v>
@@ -9713,7 +9721,7 @@
       <c r="I224" s="1"/>
       <c r="J224" s="1"/>
       <c r="K224" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L224" s="1" t="s">
         <v>25</v>
@@ -9754,13 +9762,13 @@
         <v>55</v>
       </c>
       <c r="I225" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J225" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K225" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L225" t="s">
         <v>26</v>
@@ -9799,7 +9807,7 @@
         <v>55</v>
       </c>
       <c r="K226" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L226" t="s">
         <v>27</v>
@@ -9832,7 +9840,7 @@
         <v>55</v>
       </c>
       <c r="K227" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L227" t="s">
         <v>28</v>
@@ -9862,12 +9870,12 @@
         <v>21</v>
       </c>
       <c r="H228" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I228" s="1"/>
       <c r="J228" s="1"/>
       <c r="K228" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L228" s="1" t="s">
         <v>24</v>
@@ -9903,12 +9911,12 @@
         <v>21</v>
       </c>
       <c r="H229" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I229" s="1"/>
       <c r="J229" s="1"/>
       <c r="K229" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L229" s="1" t="s">
         <v>25</v>
@@ -9944,16 +9952,16 @@
         <v>21</v>
       </c>
       <c r="H230" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I230" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J230" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K230" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L230" t="s">
         <v>26</v>
@@ -9987,10 +9995,10 @@
         <v>21</v>
       </c>
       <c r="H231" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K231" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L231" t="s">
         <v>27</v>
@@ -10021,10 +10029,10 @@
         <v>21</v>
       </c>
       <c r="H232" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K232" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L232" t="s">
         <v>28</v>
@@ -10060,7 +10068,7 @@
       <c r="I233" s="1"/>
       <c r="J233" s="1"/>
       <c r="K233" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L233" s="1" t="s">
         <v>24</v>
@@ -10103,7 +10111,7 @@
       <c r="I234" s="1"/>
       <c r="J234" s="1"/>
       <c r="K234" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L234" s="1" t="s">
         <v>25</v>
@@ -10144,13 +10152,13 @@
         <v>29</v>
       </c>
       <c r="I235" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J235" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K235" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L235" t="s">
         <v>26</v>
@@ -10189,13 +10197,13 @@
         <v>29</v>
       </c>
       <c r="I236" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J236" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K236" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L236" t="s">
         <v>27</v>
@@ -10234,7 +10242,7 @@
         <v>29</v>
       </c>
       <c r="K237" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L237" t="s">
         <v>28</v>
@@ -10264,7 +10272,7 @@
         <v>21</v>
       </c>
       <c r="H238" s="1" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I238" s="1"/>
       <c r="J238" s="1"/>
@@ -10305,7 +10313,7 @@
         <v>21</v>
       </c>
       <c r="H239" s="1" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I239" s="1"/>
       <c r="J239" s="1"/>
@@ -10346,13 +10354,13 @@
         <v>21</v>
       </c>
       <c r="H240" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I240" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J240" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K240" t="s">
         <v>33</v>
@@ -10389,7 +10397,7 @@
         <v>21</v>
       </c>
       <c r="H241" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="K241" t="s">
         <v>33</v>
@@ -10423,7 +10431,7 @@
         <v>21</v>
       </c>
       <c r="H242" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="K242" t="s">
         <v>33</v>
@@ -10542,10 +10550,10 @@
         <v>55</v>
       </c>
       <c r="I245" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J245" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K245" t="s">
         <v>33</v>
@@ -10735,10 +10743,10 @@
         <v>29</v>
       </c>
       <c r="I250" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J250" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K250" t="s">
         <v>33</v>
@@ -10843,12 +10851,12 @@
         <v>21</v>
       </c>
       <c r="H253" s="1" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I253" s="1"/>
       <c r="J253" s="1"/>
       <c r="K253" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L253" s="1" t="s">
         <v>24</v>
@@ -10884,12 +10892,12 @@
         <v>21</v>
       </c>
       <c r="H254" s="1" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I254" s="1"/>
       <c r="J254" s="1"/>
       <c r="K254" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L254" s="1" t="s">
         <v>25</v>
@@ -10925,16 +10933,16 @@
         <v>21</v>
       </c>
       <c r="H255" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I255" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J255" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K255" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L255" t="s">
         <v>26</v>
@@ -10968,10 +10976,10 @@
         <v>21</v>
       </c>
       <c r="H256" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="K256" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L256" t="s">
         <v>27</v>
@@ -11002,10 +11010,10 @@
         <v>21</v>
       </c>
       <c r="H257" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="K257" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L257" t="s">
         <v>28</v>
@@ -11036,12 +11044,12 @@
         <v>21</v>
       </c>
       <c r="H258" s="1" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I258" s="1"/>
       <c r="J258" s="1"/>
       <c r="K258" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L258" s="1" t="s">
         <v>24</v>
@@ -11077,12 +11085,12 @@
         <v>21</v>
       </c>
       <c r="H259" s="1" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I259" s="1"/>
       <c r="J259" s="1"/>
       <c r="K259" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L259" s="1" t="s">
         <v>25</v>
@@ -11118,16 +11126,16 @@
         <v>21</v>
       </c>
       <c r="H260" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I260" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J260" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K260" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L260" t="s">
         <v>26</v>
@@ -11161,10 +11169,10 @@
         <v>21</v>
       </c>
       <c r="H261" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="K261" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L261" t="s">
         <v>27</v>
@@ -11195,10 +11203,10 @@
         <v>21</v>
       </c>
       <c r="H262" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="K262" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L262" t="s">
         <v>28</v>
@@ -11234,7 +11242,7 @@
       <c r="I263" s="1"/>
       <c r="J263" s="1"/>
       <c r="K263" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L263" s="1" t="s">
         <v>24</v>
@@ -11277,7 +11285,7 @@
       <c r="I264" s="1"/>
       <c r="J264" s="1"/>
       <c r="K264" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L264" s="1" t="s">
         <v>25</v>
@@ -11318,13 +11326,13 @@
         <v>55</v>
       </c>
       <c r="I265" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J265" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K265" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L265" t="s">
         <v>26</v>
@@ -11363,7 +11371,7 @@
         <v>55</v>
       </c>
       <c r="K266" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L266" t="s">
         <v>27</v>
@@ -11396,7 +11404,7 @@
         <v>55</v>
       </c>
       <c r="K267" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L267" t="s">
         <v>28</v>
@@ -11431,7 +11439,7 @@
       <c r="I268" s="1"/>
       <c r="J268" s="1"/>
       <c r="K268" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L268" s="1" t="s">
         <v>24</v>
@@ -11472,7 +11480,7 @@
       <c r="I269" s="1"/>
       <c r="J269" s="1"/>
       <c r="K269" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L269" s="1" t="s">
         <v>25</v>
@@ -11511,13 +11519,13 @@
         <v>29</v>
       </c>
       <c r="I270" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J270" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K270" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L270" t="s">
         <v>26</v>
@@ -11554,7 +11562,7 @@
         <v>29</v>
       </c>
       <c r="K271" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L271" t="s">
         <v>27</v>
@@ -11588,7 +11596,7 @@
         <v>29</v>
       </c>
       <c r="K272" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L272" t="s">
         <v>28</v>
@@ -11624,7 +11632,7 @@
       <c r="I273" s="1"/>
       <c r="J273" s="1"/>
       <c r="K273" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L273" s="1" t="s">
         <v>24</v>
@@ -11665,7 +11673,7 @@
       <c r="I274" s="1"/>
       <c r="J274" s="1"/>
       <c r="K274" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L274" s="1" t="s">
         <v>25</v>
@@ -11704,13 +11712,13 @@
         <v>55</v>
       </c>
       <c r="I275" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J275" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K275" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L275" t="s">
         <v>26</v>
@@ -11747,7 +11755,7 @@
         <v>55</v>
       </c>
       <c r="K276" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L276" t="s">
         <v>27</v>
@@ -11781,7 +11789,7 @@
         <v>55</v>
       </c>
       <c r="K277" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L277" t="s">
         <v>28</v>
@@ -11817,7 +11825,7 @@
       <c r="I278" s="1"/>
       <c r="J278" s="1"/>
       <c r="K278" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L278" s="1" t="s">
         <v>24</v>
@@ -11858,7 +11866,7 @@
       <c r="I279" s="1"/>
       <c r="J279" s="1"/>
       <c r="K279" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L279" s="1" t="s">
         <v>25</v>
@@ -11897,13 +11905,13 @@
         <v>29</v>
       </c>
       <c r="I280" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J280" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K280" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L280" t="s">
         <v>26</v>
@@ -11940,13 +11948,13 @@
         <v>29</v>
       </c>
       <c r="I281" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J281" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K281" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L281" t="s">
         <v>27</v>
@@ -11983,7 +11991,7 @@
         <v>29</v>
       </c>
       <c r="K282" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L282" t="s">
         <v>28</v>
@@ -12019,7 +12027,7 @@
       <c r="I283" s="1"/>
       <c r="J283" s="1"/>
       <c r="K283" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L283" s="1" t="s">
         <v>24</v>
@@ -12062,7 +12070,7 @@
       <c r="I284" s="1"/>
       <c r="J284" s="1"/>
       <c r="K284" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L284" s="1" t="s">
         <v>25</v>
@@ -12103,13 +12111,13 @@
         <v>55</v>
       </c>
       <c r="I285" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J285" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K285" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L285" t="s">
         <v>26</v>
@@ -12148,7 +12156,7 @@
         <v>55</v>
       </c>
       <c r="K286" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L286" t="s">
         <v>27</v>
@@ -12181,7 +12189,7 @@
         <v>55</v>
       </c>
       <c r="K287" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L287" t="s">
         <v>28</v>
@@ -12216,7 +12224,7 @@
       <c r="I288" s="1"/>
       <c r="J288" s="1"/>
       <c r="K288" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L288" s="1" t="s">
         <v>24</v>
@@ -12257,7 +12265,7 @@
       <c r="I289" s="1"/>
       <c r="J289" s="1"/>
       <c r="K289" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L289" s="1" t="s">
         <v>25</v>
@@ -12296,13 +12304,13 @@
         <v>29</v>
       </c>
       <c r="I290" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J290" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K290" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L290" t="s">
         <v>26</v>
@@ -12339,7 +12347,7 @@
         <v>29</v>
       </c>
       <c r="K291" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L291" t="s">
         <v>27</v>
@@ -12373,7 +12381,7 @@
         <v>29</v>
       </c>
       <c r="K292" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L292" t="s">
         <v>28</v>
@@ -12404,7 +12412,7 @@
         <v>21</v>
       </c>
       <c r="H293" s="1" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I293" s="1"/>
       <c r="J293" s="1"/>
@@ -12445,7 +12453,7 @@
         <v>21</v>
       </c>
       <c r="H294" s="1" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I294" s="1"/>
       <c r="J294" s="1"/>
@@ -12486,13 +12494,13 @@
         <v>21</v>
       </c>
       <c r="H295" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I295" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J295" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K295" t="s">
         <v>34</v>
@@ -12529,7 +12537,7 @@
         <v>21</v>
       </c>
       <c r="H296" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="K296" t="s">
         <v>34</v>
@@ -12563,7 +12571,7 @@
         <v>21</v>
       </c>
       <c r="H297" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="K297" t="s">
         <v>34</v>
@@ -12597,7 +12605,7 @@
         <v>21</v>
       </c>
       <c r="H298" s="1" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I298" s="1"/>
       <c r="J298" s="1"/>
@@ -12638,7 +12646,7 @@
         <v>21</v>
       </c>
       <c r="H299" s="1" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I299" s="1"/>
       <c r="J299" s="1"/>
@@ -12679,13 +12687,13 @@
         <v>21</v>
       </c>
       <c r="H300" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I300" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J300" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K300" t="s">
         <v>34</v>
@@ -12722,7 +12730,7 @@
         <v>21</v>
       </c>
       <c r="H301" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="K301" t="s">
         <v>34</v>
@@ -12756,7 +12764,7 @@
         <v>21</v>
       </c>
       <c r="H302" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="K302" t="s">
         <v>34</v>
@@ -12875,10 +12883,10 @@
         <v>55</v>
       </c>
       <c r="I305" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J305" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K305" t="s">
         <v>34</v>
@@ -13068,10 +13076,10 @@
         <v>36</v>
       </c>
       <c r="I310" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J310" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K310" t="s">
         <v>34</v>
@@ -13261,10 +13269,10 @@
         <v>43</v>
       </c>
       <c r="I315" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J315" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K315" t="s">
         <v>34</v>
@@ -13454,10 +13462,10 @@
         <v>38</v>
       </c>
       <c r="I320" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J320" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K320" t="s">
         <v>34</v>
@@ -13647,10 +13655,10 @@
         <v>39</v>
       </c>
       <c r="I325" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J325" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K325" t="s">
         <v>34</v>
@@ -13840,10 +13848,10 @@
         <v>40</v>
       </c>
       <c r="I330" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J330" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K330" t="s">
         <v>34</v>
@@ -14037,10 +14045,10 @@
         <v>29</v>
       </c>
       <c r="I335" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J335" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K335" t="s">
         <v>34</v>
@@ -14150,7 +14158,7 @@
       <c r="I338" s="1"/>
       <c r="J338" s="1"/>
       <c r="K338" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L338" s="1" t="s">
         <v>24</v>
@@ -14191,7 +14199,7 @@
       <c r="I339" s="1"/>
       <c r="J339" s="1"/>
       <c r="K339" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L339" s="1" t="s">
         <v>25</v>
@@ -14230,13 +14238,13 @@
         <v>55</v>
       </c>
       <c r="I340" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J340" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K340" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L340" t="s">
         <v>26</v>
@@ -14273,7 +14281,7 @@
         <v>55</v>
       </c>
       <c r="K341" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L341" t="s">
         <v>27</v>
@@ -14307,7 +14315,7 @@
         <v>55</v>
       </c>
       <c r="K342" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L342" t="s">
         <v>28</v>
@@ -14343,7 +14351,7 @@
       <c r="I343" s="1"/>
       <c r="J343" s="1"/>
       <c r="K343" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L343" s="1" t="s">
         <v>24</v>
@@ -14386,7 +14394,7 @@
       <c r="I344" s="1"/>
       <c r="J344" s="1"/>
       <c r="K344" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L344" s="1" t="s">
         <v>25</v>
@@ -14427,13 +14435,13 @@
         <v>29</v>
       </c>
       <c r="I345" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J345" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K345" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L345" t="s">
         <v>26</v>
@@ -14472,13 +14480,13 @@
         <v>29</v>
       </c>
       <c r="I346" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J346" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K346" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L346" t="s">
         <v>27</v>
@@ -14517,7 +14525,7 @@
         <v>29</v>
       </c>
       <c r="K347" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L347" t="s">
         <v>28</v>
@@ -14552,7 +14560,7 @@
       <c r="I348" s="1"/>
       <c r="J348" s="1"/>
       <c r="K348" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L348" s="1" t="s">
         <v>24</v>
@@ -14593,7 +14601,7 @@
       <c r="I349" s="1"/>
       <c r="J349" s="1"/>
       <c r="K349" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L349" s="1" t="s">
         <v>25</v>
@@ -14632,13 +14640,13 @@
         <v>55</v>
       </c>
       <c r="I350" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J350" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K350" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L350" t="s">
         <v>26</v>
@@ -14675,7 +14683,7 @@
         <v>55</v>
       </c>
       <c r="K351" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L351" t="s">
         <v>27</v>
@@ -14709,7 +14717,7 @@
         <v>55</v>
       </c>
       <c r="K352" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L352" t="s">
         <v>28</v>
@@ -14745,7 +14753,7 @@
       <c r="I353" s="1"/>
       <c r="J353" s="1"/>
       <c r="K353" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L353" s="1" t="s">
         <v>24</v>
@@ -14788,7 +14796,7 @@
       <c r="I354" s="1"/>
       <c r="J354" s="1"/>
       <c r="K354" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L354" s="1" t="s">
         <v>25</v>
@@ -14829,13 +14837,13 @@
         <v>29</v>
       </c>
       <c r="I355" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J355" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K355" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L355" t="s">
         <v>26</v>
@@ -14874,13 +14882,13 @@
         <v>29</v>
       </c>
       <c r="I356" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J356" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K356" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L356" t="s">
         <v>27</v>
@@ -14919,7 +14927,7 @@
         <v>29</v>
       </c>
       <c r="K357" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L357" t="s">
         <v>28</v>
@@ -14954,7 +14962,7 @@
       <c r="I358" s="1"/>
       <c r="J358" s="1"/>
       <c r="K358" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L358" s="1" t="s">
         <v>24</v>
@@ -14995,7 +15003,7 @@
       <c r="I359" s="1"/>
       <c r="J359" s="1"/>
       <c r="K359" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L359" s="1" t="s">
         <v>25</v>
@@ -15034,13 +15042,13 @@
         <v>55</v>
       </c>
       <c r="I360" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J360" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K360" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L360" t="s">
         <v>26</v>
@@ -15077,7 +15085,7 @@
         <v>55</v>
       </c>
       <c r="K361" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L361" t="s">
         <v>27</v>
@@ -15111,7 +15119,7 @@
         <v>55</v>
       </c>
       <c r="K362" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L362" t="s">
         <v>28</v>
@@ -15147,7 +15155,7 @@
       <c r="I363" s="1"/>
       <c r="J363" s="1"/>
       <c r="K363" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L363" s="1" t="s">
         <v>24</v>
@@ -15188,7 +15196,7 @@
       <c r="I364" s="1"/>
       <c r="J364" s="1"/>
       <c r="K364" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L364" s="1" t="s">
         <v>25</v>
@@ -15227,13 +15235,13 @@
         <v>29</v>
       </c>
       <c r="I365" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J365" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K365" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L365" t="s">
         <v>26</v>
@@ -15270,13 +15278,13 @@
         <v>29</v>
       </c>
       <c r="I366" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J366" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K366" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L366" t="s">
         <v>27</v>
@@ -15313,7 +15321,7 @@
         <v>29</v>
       </c>
       <c r="K367" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L367" t="s">
         <v>28</v>
@@ -15349,7 +15357,7 @@
       <c r="I368" s="1"/>
       <c r="J368" s="1"/>
       <c r="K368" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L368" s="1" t="s">
         <v>24</v>
@@ -15390,7 +15398,7 @@
       <c r="I369" s="1"/>
       <c r="J369" s="1"/>
       <c r="K369" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L369" s="1" t="s">
         <v>25</v>
@@ -15429,13 +15437,13 @@
         <v>36</v>
       </c>
       <c r="I370" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J370" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K370" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L370" t="s">
         <v>26</v>
@@ -15472,7 +15480,7 @@
         <v>36</v>
       </c>
       <c r="K371" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L371" t="s">
         <v>27</v>
@@ -15506,7 +15514,7 @@
         <v>36</v>
       </c>
       <c r="K372" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L372" t="s">
         <v>28</v>
@@ -15542,7 +15550,7 @@
       <c r="I373" s="1"/>
       <c r="J373" s="1"/>
       <c r="K373" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L373" s="1" t="s">
         <v>24</v>
@@ -15583,7 +15591,7 @@
       <c r="I374" s="1"/>
       <c r="J374" s="1"/>
       <c r="K374" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L374" s="1" t="s">
         <v>25</v>
@@ -15622,13 +15630,13 @@
         <v>43</v>
       </c>
       <c r="I375" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J375" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K375" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L375" t="s">
         <v>26</v>
@@ -15665,7 +15673,7 @@
         <v>43</v>
       </c>
       <c r="K376" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L376" t="s">
         <v>27</v>
@@ -15699,7 +15707,7 @@
         <v>43</v>
       </c>
       <c r="K377" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L377" t="s">
         <v>28</v>
@@ -15735,7 +15743,7 @@
       <c r="I378" s="1"/>
       <c r="J378" s="1"/>
       <c r="K378" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L378" s="1" t="s">
         <v>24</v>
@@ -15776,7 +15784,7 @@
       <c r="I379" s="1"/>
       <c r="J379" s="1"/>
       <c r="K379" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L379" s="1" t="s">
         <v>25</v>
@@ -15815,13 +15823,13 @@
         <v>38</v>
       </c>
       <c r="I380" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J380" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K380" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L380" t="s">
         <v>26</v>
@@ -15858,7 +15866,7 @@
         <v>38</v>
       </c>
       <c r="K381" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L381" t="s">
         <v>27</v>
@@ -15892,7 +15900,7 @@
         <v>38</v>
       </c>
       <c r="K382" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L382" t="s">
         <v>28</v>
@@ -15928,7 +15936,7 @@
       <c r="I383" s="1"/>
       <c r="J383" s="1"/>
       <c r="K383" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L383" s="1" t="s">
         <v>24</v>
@@ -15969,7 +15977,7 @@
       <c r="I384" s="1"/>
       <c r="J384" s="1"/>
       <c r="K384" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L384" s="1" t="s">
         <v>25</v>
@@ -16008,13 +16016,13 @@
         <v>39</v>
       </c>
       <c r="I385" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J385" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K385" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L385" t="s">
         <v>26</v>
@@ -16051,7 +16059,7 @@
         <v>39</v>
       </c>
       <c r="K386" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L386" t="s">
         <v>27</v>
@@ -16085,7 +16093,7 @@
         <v>39</v>
       </c>
       <c r="K387" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L387" t="s">
         <v>28</v>
@@ -16121,7 +16129,7 @@
       <c r="I388" s="1"/>
       <c r="J388" s="1"/>
       <c r="K388" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L388" s="1" t="s">
         <v>24</v>
@@ -16162,7 +16170,7 @@
       <c r="I389" s="1"/>
       <c r="J389" s="1"/>
       <c r="K389" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L389" s="1" t="s">
         <v>25</v>
@@ -16201,13 +16209,13 @@
         <v>40</v>
       </c>
       <c r="I390" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J390" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K390" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L390" t="s">
         <v>26</v>
@@ -16244,7 +16252,7 @@
         <v>40</v>
       </c>
       <c r="K391" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L391" t="s">
         <v>27</v>
@@ -16278,7 +16286,7 @@
         <v>40</v>
       </c>
       <c r="K392" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L392" t="s">
         <v>28</v>
@@ -16314,7 +16322,7 @@
       <c r="I393" s="1"/>
       <c r="J393" s="1"/>
       <c r="K393" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L393" s="1" t="s">
         <v>24</v>
@@ -16357,7 +16365,7 @@
       <c r="I394" s="1"/>
       <c r="J394" s="1"/>
       <c r="K394" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L394" s="1" t="s">
         <v>25</v>
@@ -16398,13 +16406,13 @@
         <v>29</v>
       </c>
       <c r="I395" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J395" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K395" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L395" t="s">
         <v>26</v>
@@ -16443,13 +16451,13 @@
         <v>29</v>
       </c>
       <c r="I396" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J396" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K396" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L396" t="s">
         <v>27</v>
@@ -16488,7 +16496,7 @@
         <v>29</v>
       </c>
       <c r="K397" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L397" t="s">
         <v>28</v>
@@ -16603,10 +16611,10 @@
         <v>29</v>
       </c>
       <c r="I400" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J400" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K400" t="s">
         <v>35</v>
@@ -16646,10 +16654,10 @@
         <v>29</v>
       </c>
       <c r="I401" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J401" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K401" t="s">
         <v>35</v>
@@ -16720,7 +16728,7 @@
         <v>21</v>
       </c>
       <c r="H403" s="1" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I403" s="1"/>
       <c r="J403" s="1"/>
@@ -16761,7 +16769,7 @@
         <v>21</v>
       </c>
       <c r="H404" s="1" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I404" s="1"/>
       <c r="J404" s="1"/>
@@ -16802,13 +16810,13 @@
         <v>21</v>
       </c>
       <c r="H405" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I405" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J405" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K405" t="s">
         <v>37</v>
@@ -16845,7 +16853,7 @@
         <v>21</v>
       </c>
       <c r="H406" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="K406" t="s">
         <v>37</v>
@@ -16879,7 +16887,7 @@
         <v>21</v>
       </c>
       <c r="H407" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="K407" t="s">
         <v>37</v>
@@ -16913,7 +16921,7 @@
         <v>21</v>
       </c>
       <c r="H408" s="1" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I408" s="1"/>
       <c r="J408" s="1"/>
@@ -16954,7 +16962,7 @@
         <v>21</v>
       </c>
       <c r="H409" s="1" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I409" s="1"/>
       <c r="J409" s="1"/>
@@ -16995,13 +17003,13 @@
         <v>21</v>
       </c>
       <c r="H410" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I410" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J410" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K410" t="s">
         <v>37</v>
@@ -17038,7 +17046,7 @@
         <v>21</v>
       </c>
       <c r="H411" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="K411" t="s">
         <v>37</v>
@@ -17072,7 +17080,7 @@
         <v>21</v>
       </c>
       <c r="H412" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="K412" t="s">
         <v>37</v>
@@ -17191,10 +17199,10 @@
         <v>55</v>
       </c>
       <c r="I415" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J415" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K415" t="s">
         <v>37</v>
@@ -17384,10 +17392,10 @@
         <v>38</v>
       </c>
       <c r="I420" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J420" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K420" t="s">
         <v>37</v>
@@ -17577,10 +17585,10 @@
         <v>39</v>
       </c>
       <c r="I425" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J425" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K425" t="s">
         <v>37</v>
@@ -17774,10 +17782,10 @@
         <v>40</v>
       </c>
       <c r="I430" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J430" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K430" t="s">
         <v>37</v>
@@ -17882,7 +17890,7 @@
         <v>21</v>
       </c>
       <c r="H433" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I433" s="1"/>
       <c r="J433" s="1"/>
@@ -17923,7 +17931,7 @@
         <v>21</v>
       </c>
       <c r="H434" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I434" s="1"/>
       <c r="J434" s="1"/>
@@ -17964,13 +17972,13 @@
         <v>21</v>
       </c>
       <c r="H435" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I435" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J435" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K435" t="s">
         <v>37</v>
@@ -18007,7 +18015,7 @@
         <v>21</v>
       </c>
       <c r="H436" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K436" t="s">
         <v>37</v>
@@ -18041,7 +18049,7 @@
         <v>21</v>
       </c>
       <c r="H437" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K437" t="s">
         <v>37</v>
@@ -18164,10 +18172,10 @@
         <v>41</v>
       </c>
       <c r="I440" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J440" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K440" t="s">
         <v>37</v>
@@ -18361,10 +18369,10 @@
         <v>29</v>
       </c>
       <c r="I445" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J445" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K445" t="s">
         <v>37</v>
@@ -18406,10 +18414,10 @@
         <v>29</v>
       </c>
       <c r="I446" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J446" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K446" t="s">
         <v>37</v>
@@ -18481,12 +18489,12 @@
         <v>21</v>
       </c>
       <c r="H448" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I448" s="1"/>
       <c r="J448" s="1"/>
       <c r="K448" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L448" s="1" t="s">
         <v>24</v>
@@ -18524,12 +18532,12 @@
         <v>21</v>
       </c>
       <c r="H449" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I449" s="1"/>
       <c r="J449" s="1"/>
       <c r="K449" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L449" s="1" t="s">
         <v>25</v>
@@ -18567,16 +18575,16 @@
         <v>21</v>
       </c>
       <c r="H450" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I450" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J450" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K450" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L450" t="s">
         <v>26</v>
@@ -18612,10 +18620,10 @@
         <v>21</v>
       </c>
       <c r="H451" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K451" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L451" t="s">
         <v>27</v>
@@ -18645,10 +18653,10 @@
         <v>21</v>
       </c>
       <c r="H452" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K452" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L452" t="s">
         <v>28</v>
@@ -18767,10 +18775,10 @@
         <v>43</v>
       </c>
       <c r="I455" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J455" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K455" t="s">
         <v>44</v>
@@ -18812,10 +18820,10 @@
         <v>43</v>
       </c>
       <c r="I456" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J456" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K456" t="s">
         <v>44</v>
@@ -18976,10 +18984,10 @@
         <v>39</v>
       </c>
       <c r="I460" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J460" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K460" t="s">
         <v>44</v>
@@ -19021,10 +19029,10 @@
         <v>39</v>
       </c>
       <c r="I461" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J461" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K461" t="s">
         <v>44</v>
@@ -19181,10 +19189,10 @@
         <v>40</v>
       </c>
       <c r="I465" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J465" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K465" t="s">
         <v>44</v>
@@ -19374,10 +19382,10 @@
         <v>29</v>
       </c>
       <c r="I470" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J470" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K470" t="s">
         <v>44</v>
@@ -19482,7 +19490,7 @@
         <v>21</v>
       </c>
       <c r="H473" s="1" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I473" s="1"/>
       <c r="J473" s="1"/>
@@ -19523,7 +19531,7 @@
         <v>21</v>
       </c>
       <c r="H474" s="1" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I474" s="1"/>
       <c r="J474" s="1"/>
@@ -19564,13 +19572,13 @@
         <v>21</v>
       </c>
       <c r="H475" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I475" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J475" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K475" t="s">
         <v>45</v>
@@ -19607,7 +19615,7 @@
         <v>21</v>
       </c>
       <c r="H476" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="K476" t="s">
         <v>45</v>
@@ -19641,7 +19649,7 @@
         <v>21</v>
       </c>
       <c r="H477" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="K477" t="s">
         <v>45</v>
@@ -19760,10 +19768,10 @@
         <v>36</v>
       </c>
       <c r="I480" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J480" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K480" t="s">
         <v>45</v>
@@ -19953,10 +19961,10 @@
         <v>43</v>
       </c>
       <c r="I485" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J485" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K485" t="s">
         <v>45</v>
@@ -20146,10 +20154,10 @@
         <v>39</v>
       </c>
       <c r="I490" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J490" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K490" t="s">
         <v>45</v>
@@ -20339,10 +20347,10 @@
         <v>40</v>
       </c>
       <c r="I495" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J495" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K495" t="s">
         <v>45</v>
@@ -20536,10 +20544,10 @@
         <v>29</v>
       </c>
       <c r="I500" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J500" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K500" t="s">
         <v>45</v>
@@ -20581,10 +20589,10 @@
         <v>29</v>
       </c>
       <c r="I501" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J501" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K501" t="s">
         <v>45</v>
@@ -20661,7 +20669,7 @@
       <c r="I503" s="1"/>
       <c r="J503" s="1"/>
       <c r="K503" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L503" s="1" t="s">
         <v>24</v>
@@ -20702,7 +20710,7 @@
       <c r="I504" s="1"/>
       <c r="J504" s="1"/>
       <c r="K504" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L504" s="1" t="s">
         <v>25</v>
@@ -20741,13 +20749,13 @@
         <v>29</v>
       </c>
       <c r="I505" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J505" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K505" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L505" t="s">
         <v>26</v>
@@ -20784,7 +20792,7 @@
         <v>29</v>
       </c>
       <c r="K506" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L506" t="s">
         <v>27</v>
@@ -20818,7 +20826,7 @@
         <v>29</v>
       </c>
       <c r="K507" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L507" t="s">
         <v>28</v>
@@ -20854,7 +20862,7 @@
       <c r="I508" s="1"/>
       <c r="J508" s="1"/>
       <c r="K508" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L508" s="1" t="s">
         <v>24</v>
@@ -20895,7 +20903,7 @@
       <c r="I509" s="1"/>
       <c r="J509" s="1"/>
       <c r="K509" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L509" s="1" t="s">
         <v>25</v>
@@ -20934,13 +20942,13 @@
         <v>36</v>
       </c>
       <c r="I510" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J510" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K510" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L510" t="s">
         <v>26</v>
@@ -20977,7 +20985,7 @@
         <v>36</v>
       </c>
       <c r="K511" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L511" t="s">
         <v>27</v>
@@ -21011,7 +21019,7 @@
         <v>36</v>
       </c>
       <c r="K512" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L512" t="s">
         <v>28</v>
@@ -21047,7 +21055,7 @@
       <c r="I513" s="1"/>
       <c r="J513" s="1"/>
       <c r="K513" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L513" s="1" t="s">
         <v>24</v>
@@ -21088,7 +21096,7 @@
       <c r="I514" s="1"/>
       <c r="J514" s="1"/>
       <c r="K514" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L514" s="1" t="s">
         <v>25</v>
@@ -21127,13 +21135,13 @@
         <v>38</v>
       </c>
       <c r="I515" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J515" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K515" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L515" t="s">
         <v>26</v>
@@ -21170,13 +21178,13 @@
         <v>38</v>
       </c>
       <c r="I516" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J516" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K516" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L516" t="s">
         <v>27</v>
@@ -21213,7 +21221,7 @@
         <v>38</v>
       </c>
       <c r="K517" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L517" t="s">
         <v>28</v>
@@ -21249,7 +21257,7 @@
       <c r="I518" s="1"/>
       <c r="J518" s="1"/>
       <c r="K518" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L518" s="1" t="s">
         <v>24</v>
@@ -21292,7 +21300,7 @@
       <c r="I519" s="1"/>
       <c r="J519" s="1"/>
       <c r="K519" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L519" s="1" t="s">
         <v>25</v>
@@ -21333,13 +21341,13 @@
         <v>29</v>
       </c>
       <c r="I520" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J520" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K520" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L520" t="s">
         <v>26</v>
@@ -21378,7 +21386,7 @@
         <v>29</v>
       </c>
       <c r="K521" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L521" t="s">
         <v>27</v>
@@ -21411,7 +21419,7 @@
         <v>29</v>
       </c>
       <c r="K522" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L522" t="s">
         <v>28</v>
@@ -21441,7 +21449,7 @@
         <v>21</v>
       </c>
       <c r="H523" s="1" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I523" s="1"/>
       <c r="J523" s="1"/>
@@ -21482,7 +21490,7 @@
         <v>21</v>
       </c>
       <c r="H524" s="1" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I524" s="1"/>
       <c r="J524" s="1"/>
@@ -21523,13 +21531,13 @@
         <v>21</v>
       </c>
       <c r="H525" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I525" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J525" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K525" t="s">
         <v>48</v>
@@ -21566,7 +21574,7 @@
         <v>21</v>
       </c>
       <c r="H526" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="K526" t="s">
         <v>48</v>
@@ -21600,7 +21608,7 @@
         <v>21</v>
       </c>
       <c r="H527" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="K527" t="s">
         <v>48</v>
@@ -21634,7 +21642,7 @@
         <v>21</v>
       </c>
       <c r="H528" s="1" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I528" s="1"/>
       <c r="J528" s="1"/>
@@ -21675,7 +21683,7 @@
         <v>21</v>
       </c>
       <c r="H529" s="1" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I529" s="1"/>
       <c r="J529" s="1"/>
@@ -21716,13 +21724,13 @@
         <v>21</v>
       </c>
       <c r="H530" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I530" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J530" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K530" t="s">
         <v>48</v>
@@ -21759,7 +21767,7 @@
         <v>21</v>
       </c>
       <c r="H531" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="K531" t="s">
         <v>48</v>
@@ -21793,7 +21801,7 @@
         <v>21</v>
       </c>
       <c r="H532" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="K532" t="s">
         <v>48</v>
@@ -21916,10 +21924,10 @@
         <v>55</v>
       </c>
       <c r="I535" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J535" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K535" t="s">
         <v>48</v>
@@ -22109,10 +22117,10 @@
         <v>36</v>
       </c>
       <c r="I540" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J540" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K540" t="s">
         <v>48</v>
@@ -22152,10 +22160,10 @@
         <v>36</v>
       </c>
       <c r="I541" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J541" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K541" t="s">
         <v>48</v>
@@ -22311,10 +22319,10 @@
         <v>43</v>
       </c>
       <c r="I545" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J545" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K545" t="s">
         <v>48</v>
@@ -22504,10 +22512,10 @@
         <v>38</v>
       </c>
       <c r="I550" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J550" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K550" t="s">
         <v>48</v>
@@ -22697,10 +22705,10 @@
         <v>39</v>
       </c>
       <c r="I555" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J555" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K555" t="s">
         <v>48</v>
@@ -22890,10 +22898,10 @@
         <v>40</v>
       </c>
       <c r="I560" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J560" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K560" t="s">
         <v>48</v>
@@ -23087,10 +23095,10 @@
         <v>41</v>
       </c>
       <c r="I565" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J565" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K565" t="s">
         <v>48</v>
@@ -23132,10 +23140,10 @@
         <v>41</v>
       </c>
       <c r="I566" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J566" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K566" t="s">
         <v>48</v>
@@ -23296,10 +23304,10 @@
         <v>49</v>
       </c>
       <c r="I570" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J570" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K570" t="s">
         <v>48</v>
@@ -23493,10 +23501,10 @@
         <v>29</v>
       </c>
       <c r="I575" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J575" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K575" t="s">
         <v>48</v>
@@ -23538,10 +23546,10 @@
         <v>29</v>
       </c>
       <c r="I576" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J576" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K576" t="s">
         <v>48</v>
@@ -23583,10 +23591,10 @@
         <v>29</v>
       </c>
       <c r="I577" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J577" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K577" t="s">
         <v>48</v>
@@ -23625,7 +23633,7 @@
         <v>21</v>
       </c>
       <c r="H578" s="1" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I578" s="1"/>
       <c r="J578" s="1"/>
@@ -23666,7 +23674,7 @@
         <v>21</v>
       </c>
       <c r="H579" s="1" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I579" s="1"/>
       <c r="J579" s="1"/>
@@ -23707,13 +23715,13 @@
         <v>21</v>
       </c>
       <c r="H580" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I580" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J580" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K580" t="s">
         <v>50</v>
@@ -23750,7 +23758,7 @@
         <v>21</v>
       </c>
       <c r="H581" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="K581" t="s">
         <v>50</v>
@@ -23784,7 +23792,7 @@
         <v>21</v>
       </c>
       <c r="H582" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="K582" t="s">
         <v>50</v>
@@ -23818,7 +23826,7 @@
         <v>21</v>
       </c>
       <c r="H583" s="1" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I583" s="1"/>
       <c r="J583" s="1"/>
@@ -23859,7 +23867,7 @@
         <v>21</v>
       </c>
       <c r="H584" s="1" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I584" s="1"/>
       <c r="J584" s="1"/>
@@ -23900,13 +23908,13 @@
         <v>21</v>
       </c>
       <c r="H585" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I585" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J585" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K585" t="s">
         <v>50</v>
@@ -23943,7 +23951,7 @@
         <v>21</v>
       </c>
       <c r="H586" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="K586" t="s">
         <v>50</v>
@@ -23977,7 +23985,7 @@
         <v>21</v>
       </c>
       <c r="H587" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="K587" t="s">
         <v>50</v>
@@ -24100,10 +24108,10 @@
         <v>55</v>
       </c>
       <c r="I590" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J590" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K590" t="s">
         <v>50</v>
@@ -24293,10 +24301,10 @@
         <v>36</v>
       </c>
       <c r="I595" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J595" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K595" t="s">
         <v>50</v>
@@ -24486,10 +24494,10 @@
         <v>43</v>
       </c>
       <c r="I600" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J600" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K600" t="s">
         <v>50</v>
@@ -24679,10 +24687,10 @@
         <v>38</v>
       </c>
       <c r="I605" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J605" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K605" t="s">
         <v>50</v>
@@ -24872,10 +24880,10 @@
         <v>39</v>
       </c>
       <c r="I610" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J610" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K610" t="s">
         <v>50</v>
@@ -25065,10 +25073,10 @@
         <v>40</v>
       </c>
       <c r="I615" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J615" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K615" t="s">
         <v>50</v>
@@ -25262,10 +25270,10 @@
         <v>29</v>
       </c>
       <c r="I620" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J620" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K620" t="s">
         <v>50</v>
@@ -25307,10 +25315,10 @@
         <v>29</v>
       </c>
       <c r="I621" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J621" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K621" t="s">
         <v>50</v>
@@ -25382,7 +25390,7 @@
         <v>21</v>
       </c>
       <c r="H623" s="1" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I623" s="1"/>
       <c r="J623" s="1"/>
@@ -25423,7 +25431,7 @@
         <v>21</v>
       </c>
       <c r="H624" s="1" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I624" s="1"/>
       <c r="J624" s="1"/>
@@ -25464,13 +25472,13 @@
         <v>21</v>
       </c>
       <c r="H625" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="I625" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J625" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K625" t="s">
         <v>51</v>
@@ -25507,7 +25515,7 @@
         <v>21</v>
       </c>
       <c r="H626" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="K626" t="s">
         <v>51</v>
@@ -25541,7 +25549,7 @@
         <v>21</v>
       </c>
       <c r="H627" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="K627" t="s">
         <v>51</v>
@@ -25575,7 +25583,7 @@
         <v>21</v>
       </c>
       <c r="H628" s="1" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I628" s="1"/>
       <c r="J628" s="1"/>
@@ -25616,7 +25624,7 @@
         <v>21</v>
       </c>
       <c r="H629" s="1" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I629" s="1"/>
       <c r="J629" s="1"/>
@@ -25657,13 +25665,13 @@
         <v>21</v>
       </c>
       <c r="H630" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="I630" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J630" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K630" t="s">
         <v>51</v>
@@ -25700,7 +25708,7 @@
         <v>21</v>
       </c>
       <c r="H631" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="K631" t="s">
         <v>51</v>
@@ -25734,7 +25742,7 @@
         <v>21</v>
       </c>
       <c r="H632" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="K632" t="s">
         <v>51</v>
@@ -25853,10 +25861,10 @@
         <v>36</v>
       </c>
       <c r="I635" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J635" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K635" t="s">
         <v>51</v>
@@ -26046,10 +26054,10 @@
         <v>43</v>
       </c>
       <c r="I640" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J640" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K640" t="s">
         <v>51</v>
@@ -26089,10 +26097,10 @@
         <v>43</v>
       </c>
       <c r="I641" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J641" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K641" t="s">
         <v>51</v>
@@ -26248,10 +26256,10 @@
         <v>38</v>
       </c>
       <c r="I645" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J645" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K645" t="s">
         <v>51</v>
@@ -26445,10 +26453,10 @@
         <v>39</v>
       </c>
       <c r="I650" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J650" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K650" t="s">
         <v>51</v>
@@ -26638,10 +26646,10 @@
         <v>40</v>
       </c>
       <c r="I655" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J655" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K655" t="s">
         <v>51</v>
@@ -26831,10 +26839,10 @@
         <v>29</v>
       </c>
       <c r="I660" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J660" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K660" t="s">
         <v>51</v>
@@ -26874,10 +26882,10 @@
         <v>29</v>
       </c>
       <c r="I661" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J661" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K661" t="s">
         <v>51</v>
@@ -27033,10 +27041,10 @@
         <v>39</v>
       </c>
       <c r="I665" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J665" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K665" t="s">
         <v>52</v>
@@ -27226,10 +27234,10 @@
         <v>40</v>
       </c>
       <c r="I670" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J670" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K670" t="s">
         <v>52</v>
@@ -27339,7 +27347,7 @@
       <c r="I673" s="1"/>
       <c r="J673" s="1"/>
       <c r="K673" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L673" s="1" t="s">
         <v>24</v>
@@ -27380,7 +27388,7 @@
       <c r="I674" s="1"/>
       <c r="J674" s="1"/>
       <c r="K674" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L674" s="1" t="s">
         <v>25</v>
@@ -27419,13 +27427,13 @@
         <v>36</v>
       </c>
       <c r="I675" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J675" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K675" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L675" t="s">
         <v>26</v>
@@ -27462,7 +27470,7 @@
         <v>36</v>
       </c>
       <c r="K676" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L676" t="s">
         <v>27</v>
@@ -27496,7 +27504,7 @@
         <v>36</v>
       </c>
       <c r="K677" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L677" t="s">
         <v>28</v>
@@ -27532,7 +27540,7 @@
       <c r="I678" s="1"/>
       <c r="J678" s="1"/>
       <c r="K678" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L678" s="1" t="s">
         <v>24</v>
@@ -27575,7 +27583,7 @@
       <c r="I679" s="1"/>
       <c r="J679" s="1"/>
       <c r="K679" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L679" s="1" t="s">
         <v>25</v>
@@ -27616,13 +27624,13 @@
         <v>38</v>
       </c>
       <c r="I680" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J680" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K680" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L680" t="s">
         <v>26</v>
@@ -27661,7 +27669,7 @@
         <v>38</v>
       </c>
       <c r="K681" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L681" t="s">
         <v>27</v>
@@ -27694,7 +27702,7 @@
         <v>38</v>
       </c>
       <c r="K682" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L682" t="s">
         <v>28</v>
@@ -27729,7 +27737,7 @@
       <c r="I683" s="1"/>
       <c r="J683" s="1"/>
       <c r="K683" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L683" s="1" t="s">
         <v>24</v>
@@ -27770,7 +27778,7 @@
       <c r="I684" s="1"/>
       <c r="J684" s="1"/>
       <c r="K684" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L684" s="1" t="s">
         <v>25</v>
@@ -27809,13 +27817,13 @@
         <v>39</v>
       </c>
       <c r="I685" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J685" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K685" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L685" t="s">
         <v>26</v>
@@ -27852,7 +27860,7 @@
         <v>39</v>
       </c>
       <c r="K686" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L686" t="s">
         <v>27</v>
@@ -27886,7 +27894,7 @@
         <v>39</v>
       </c>
       <c r="K687" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L687" t="s">
         <v>28</v>
@@ -27922,7 +27930,7 @@
       <c r="I688" s="1"/>
       <c r="J688" s="1"/>
       <c r="K688" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L688" s="1" t="s">
         <v>24</v>
@@ -27965,7 +27973,7 @@
       <c r="I689" s="1"/>
       <c r="J689" s="1"/>
       <c r="K689" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L689" s="1" t="s">
         <v>25</v>
@@ -28006,13 +28014,13 @@
         <v>29</v>
       </c>
       <c r="I690" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J690" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K690" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L690" t="s">
         <v>26</v>
@@ -28051,13 +28059,13 @@
         <v>29</v>
       </c>
       <c r="I691" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J691" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K691" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L691" t="s">
         <v>27</v>
@@ -28096,12 +28104,45 @@
         <v>29</v>
       </c>
       <c r="K692" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L692" t="s">
         <v>28</v>
       </c>
       <c r="M692" s="3"/>
+    </row>
+    <row r="693" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A693" t="s">
+        <v>53</v>
+      </c>
+      <c r="B693" t="s">
+        <v>16</v>
+      </c>
+      <c r="C693" t="s">
+        <v>17</v>
+      </c>
+      <c r="D693" t="s">
+        <v>18</v>
+      </c>
+      <c r="E693" t="s">
+        <v>31</v>
+      </c>
+      <c r="F693" t="s">
+        <v>47</v>
+      </c>
+      <c r="G693" t="s">
+        <v>21</v>
+      </c>
+      <c r="H693" t="s">
+        <v>29</v>
+      </c>
+      <c r="K693" t="s">
+        <v>74</v>
+      </c>
+      <c r="L693" t="s">
+        <v>93</v>
+      </c>
+      <c r="M693" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>